<commit_message>
Update Geocercas.xlsx and main.py
</commit_message>
<xml_diff>
--- a/data/Geocercas.xlsx
+++ b/data/Geocercas.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jlorenzini\Desktop\Logistica S.A\SCRIPTS\etl-geocercasSPMK\project-app\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B0024CD-5788-47A9-B77B-CDF73453C55D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{689C243F-F5E7-404A-AFDD-99E1CF4BC937}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-16310" windowWidth="29020" windowHeight="15700" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="360" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Geocercas" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,20 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Geocercas!$A$1:$G$541</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Rutas!$A$1:$C$1</definedName>
   </definedNames>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -5441,11 +5454,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:G541"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="E542" sqref="E542"/>
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5477,7 +5489,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>9</v>
       </c>
@@ -5500,7 +5512,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>14</v>
       </c>
@@ -5523,7 +5535,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>17</v>
       </c>
@@ -5546,7 +5558,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>21</v>
       </c>
@@ -5569,7 +5581,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>25</v>
       </c>
@@ -5592,7 +5604,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
         <v>29</v>
       </c>
@@ -5615,7 +5627,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
         <v>32</v>
       </c>
@@ -5638,7 +5650,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
         <v>35</v>
       </c>
@@ -5661,7 +5673,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
         <v>39</v>
       </c>
@@ -5684,7 +5696,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="s">
         <v>42</v>
       </c>
@@ -5707,7 +5719,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="12" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A12" s="2" t="s">
         <v>45</v>
       </c>
@@ -5730,7 +5742,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
         <v>48</v>
       </c>
@@ -5753,7 +5765,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A14" s="2" t="s">
         <v>51</v>
       </c>
@@ -5776,7 +5788,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A15" s="2" t="s">
         <v>54</v>
       </c>
@@ -5799,7 +5811,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A16" s="2" t="s">
         <v>57</v>
       </c>
@@ -5822,7 +5834,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A17" s="2" t="s">
         <v>60</v>
       </c>
@@ -5845,7 +5857,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A18" s="2" t="s">
         <v>64</v>
       </c>
@@ -5868,7 +5880,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A19" s="2" t="s">
         <v>67</v>
       </c>
@@ -5891,7 +5903,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A20" s="2" t="s">
         <v>71</v>
       </c>
@@ -5914,7 +5926,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A21" s="2" t="s">
         <v>74</v>
       </c>
@@ -5937,7 +5949,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A22" s="2" t="s">
         <v>77</v>
       </c>
@@ -5960,7 +5972,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A23" s="2" t="s">
         <v>80</v>
       </c>
@@ -5983,7 +5995,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A24" s="2" t="s">
         <v>84</v>
       </c>
@@ -6006,7 +6018,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A25" s="2" t="s">
         <v>87</v>
       </c>
@@ -6029,7 +6041,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A26" s="2" t="s">
         <v>90</v>
       </c>
@@ -6052,7 +6064,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A27" s="2" t="s">
         <v>93</v>
       </c>
@@ -6075,7 +6087,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="28" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A28" s="2" t="s">
         <v>97</v>
       </c>
@@ -6098,7 +6110,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="29" spans="1:7" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A29" s="2" t="s">
         <v>101</v>
       </c>
@@ -6121,7 +6133,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="30" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A30" s="2" t="s">
         <v>104</v>
       </c>
@@ -6144,7 +6156,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="31" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A31" s="2" t="s">
         <v>107</v>
       </c>
@@ -6167,7 +6179,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="32" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A32" s="2" t="s">
         <v>110</v>
       </c>
@@ -6190,7 +6202,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="33" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A33" s="2" t="s">
         <v>114</v>
       </c>
@@ -6213,7 +6225,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="34" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A34" s="2" t="s">
         <v>117</v>
       </c>
@@ -6236,7 +6248,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="35" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A35" s="2" t="s">
         <v>120</v>
       </c>
@@ -6259,7 +6271,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="36" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A36" s="2" t="s">
         <v>123</v>
       </c>
@@ -6282,7 +6294,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="37" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A37" s="2" t="s">
         <v>126</v>
       </c>
@@ -6305,7 +6317,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="38" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A38" s="2" t="s">
         <v>130</v>
       </c>
@@ -6328,7 +6340,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="39" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A39" s="2" t="s">
         <v>134</v>
       </c>
@@ -6351,7 +6363,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="40" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A40" s="2" t="s">
         <v>137</v>
       </c>
@@ -6374,7 +6386,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="41" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A41" s="2" t="s">
         <v>140</v>
       </c>
@@ -6397,7 +6409,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="42" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A42" s="2" t="s">
         <v>143</v>
       </c>
@@ -6420,7 +6432,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="43" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A43" s="2" t="s">
         <v>147</v>
       </c>
@@ -6443,7 +6455,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="44" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A44" s="2" t="s">
         <v>150</v>
       </c>
@@ -6466,7 +6478,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="45" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A45" s="2" t="s">
         <v>153</v>
       </c>
@@ -6489,7 +6501,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="46" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A46" s="2" t="s">
         <v>156</v>
       </c>
@@ -6512,7 +6524,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="47" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A47" s="2" t="s">
         <v>159</v>
       </c>
@@ -6535,7 +6547,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="48" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A48" s="2" t="s">
         <v>162</v>
       </c>
@@ -6558,7 +6570,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="49" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A49" s="2" t="s">
         <v>165</v>
       </c>
@@ -6581,7 +6593,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="50" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A50" s="2" t="s">
         <v>168</v>
       </c>
@@ -6604,7 +6616,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="51" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A51" s="2" t="s">
         <v>171</v>
       </c>
@@ -6627,7 +6639,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="52" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A52" s="2" t="s">
         <v>175</v>
       </c>
@@ -6650,7 +6662,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="53" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A53" s="2" t="s">
         <v>178</v>
       </c>
@@ -6673,7 +6685,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="54" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A54" s="2" t="s">
         <v>181</v>
       </c>
@@ -6696,7 +6708,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="55" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A55" s="2" t="s">
         <v>184</v>
       </c>
@@ -6719,7 +6731,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="56" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A56" s="2" t="s">
         <v>187</v>
       </c>
@@ -6742,7 +6754,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="57" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A57" s="2" t="s">
         <v>190</v>
       </c>
@@ -6765,7 +6777,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="58" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A58" s="2" t="s">
         <v>193</v>
       </c>
@@ -6788,7 +6800,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="59" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A59" s="2" t="s">
         <v>196</v>
       </c>
@@ -6811,7 +6823,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="60" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A60" s="2" t="s">
         <v>199</v>
       </c>
@@ -6834,7 +6846,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="61" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A61" s="2" t="s">
         <v>202</v>
       </c>
@@ -6857,7 +6869,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="62" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A62" s="2" t="s">
         <v>205</v>
       </c>
@@ -6880,7 +6892,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="63" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A63" s="2" t="s">
         <v>208</v>
       </c>
@@ -6903,7 +6915,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="64" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A64" s="2" t="s">
         <v>211</v>
       </c>
@@ -6926,7 +6938,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="65" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A65" s="2" t="s">
         <v>214</v>
       </c>
@@ -6949,7 +6961,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="66" spans="1:7" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A66" s="2" t="s">
         <v>217</v>
       </c>
@@ -6972,7 +6984,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="67" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A67" s="2" t="s">
         <v>220</v>
       </c>
@@ -6995,7 +7007,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="68" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A68" s="2" t="s">
         <v>223</v>
       </c>
@@ -7018,7 +7030,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="69" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A69" s="2" t="s">
         <v>227</v>
       </c>
@@ -7041,7 +7053,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="70" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A70" s="2" t="s">
         <v>230</v>
       </c>
@@ -7064,7 +7076,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="71" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A71" s="2" t="s">
         <v>233</v>
       </c>
@@ -7087,7 +7099,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="72" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A72" s="2" t="s">
         <v>236</v>
       </c>
@@ -7110,7 +7122,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="73" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A73" s="2" t="s">
         <v>239</v>
       </c>
@@ -7133,7 +7145,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="74" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A74" s="2" t="s">
         <v>243</v>
       </c>
@@ -7156,7 +7168,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="75" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A75" s="2" t="s">
         <v>246</v>
       </c>
@@ -7179,7 +7191,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="76" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A76" s="2" t="s">
         <v>249</v>
       </c>
@@ -7202,7 +7214,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="77" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A77" s="2" t="s">
         <v>252</v>
       </c>
@@ -7225,7 +7237,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="78" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A78" s="2" t="s">
         <v>255</v>
       </c>
@@ -7248,7 +7260,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="79" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A79" s="2" t="s">
         <v>258</v>
       </c>
@@ -7271,7 +7283,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="80" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A80" s="2" t="s">
         <v>261</v>
       </c>
@@ -7294,7 +7306,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="81" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A81" s="2" t="s">
         <v>265</v>
       </c>
@@ -7317,7 +7329,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="82" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A82" s="2" t="s">
         <v>268</v>
       </c>
@@ -7340,7 +7352,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="83" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A83" s="2" t="s">
         <v>271</v>
       </c>
@@ -7363,7 +7375,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="84" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A84" s="2" t="s">
         <v>274</v>
       </c>
@@ -7386,7 +7398,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="85" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A85" s="2" t="s">
         <v>277</v>
       </c>
@@ -7409,7 +7421,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="86" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A86" s="2" t="s">
         <v>281</v>
       </c>
@@ -7432,7 +7444,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="87" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A87" s="2" t="s">
         <v>284</v>
       </c>
@@ -7455,7 +7467,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="88" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A88" s="2" t="s">
         <v>287</v>
       </c>
@@ -7478,7 +7490,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="89" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A89" s="2" t="s">
         <v>290</v>
       </c>
@@ -7501,7 +7513,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="90" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A90" s="2" t="s">
         <v>293</v>
       </c>
@@ -7524,7 +7536,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="91" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A91" s="2" t="s">
         <v>296</v>
       </c>
@@ -7547,7 +7559,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="92" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A92" s="2" t="s">
         <v>300</v>
       </c>
@@ -7570,7 +7582,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="93" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A93" s="2" t="s">
         <v>303</v>
       </c>
@@ -7593,7 +7605,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="94" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A94" s="2" t="s">
         <v>306</v>
       </c>
@@ -7616,7 +7628,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="95" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A95" s="2" t="s">
         <v>309</v>
       </c>
@@ -7639,7 +7651,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="96" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A96" s="2" t="s">
         <v>312</v>
       </c>
@@ -7662,7 +7674,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="97" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A97" s="2" t="s">
         <v>315</v>
       </c>
@@ -7685,7 +7697,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="98" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A98" s="2" t="s">
         <v>318</v>
       </c>
@@ -7708,7 +7720,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="99" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A99" s="2" t="s">
         <v>322</v>
       </c>
@@ -7731,7 +7743,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="100" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A100" s="2" t="s">
         <v>325</v>
       </c>
@@ -7754,7 +7766,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="101" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A101" s="2" t="s">
         <v>328</v>
       </c>
@@ -7777,7 +7789,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="102" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A102" s="2" t="s">
         <v>331</v>
       </c>
@@ -7800,7 +7812,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="103" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A103" s="2" t="s">
         <v>334</v>
       </c>
@@ -7823,7 +7835,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="104" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A104" s="2" t="s">
         <v>337</v>
       </c>
@@ -7846,7 +7858,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="105" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A105" s="2" t="s">
         <v>340</v>
       </c>
@@ -7869,7 +7881,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="106" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A106" s="2" t="s">
         <v>343</v>
       </c>
@@ -7892,7 +7904,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="107" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A107" s="2" t="s">
         <v>346</v>
       </c>
@@ -7915,7 +7927,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="108" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A108" s="2" t="s">
         <v>349</v>
       </c>
@@ -7938,7 +7950,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="109" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A109" s="2" t="s">
         <v>352</v>
       </c>
@@ -7961,7 +7973,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="110" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A110" s="2" t="s">
         <v>355</v>
       </c>
@@ -7984,7 +7996,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="111" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A111" s="2" t="s">
         <v>358</v>
       </c>
@@ -8007,7 +8019,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="112" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A112" s="2" t="s">
         <v>361</v>
       </c>
@@ -8030,7 +8042,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="113" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A113" s="2" t="s">
         <v>364</v>
       </c>
@@ -8053,7 +8065,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="114" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A114" s="2" t="s">
         <v>367</v>
       </c>
@@ -8076,7 +8088,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="115" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A115" s="2" t="s">
         <v>370</v>
       </c>
@@ -8122,7 +8134,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="117" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A117" s="2" t="s">
         <v>375</v>
       </c>
@@ -8145,7 +8157,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="118" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A118" s="2" t="s">
         <v>378</v>
       </c>
@@ -8168,7 +8180,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="119" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A119" s="2" t="s">
         <v>381</v>
       </c>
@@ -8191,7 +8203,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="120" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A120" s="2" t="s">
         <v>384</v>
       </c>
@@ -8214,7 +8226,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="121" spans="1:7" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A121" s="2" t="s">
         <v>387</v>
       </c>
@@ -8237,7 +8249,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="122" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A122" s="2" t="s">
         <v>390</v>
       </c>
@@ -8260,7 +8272,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="123" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A123" s="2" t="s">
         <v>393</v>
       </c>
@@ -8283,7 +8295,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="124" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A124" s="2" t="s">
         <v>396</v>
       </c>
@@ -8306,7 +8318,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="125" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A125" s="2" t="s">
         <v>399</v>
       </c>
@@ -8329,7 +8341,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="126" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A126" s="2" t="s">
         <v>402</v>
       </c>
@@ -8352,7 +8364,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="127" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A127" s="2" t="s">
         <v>405</v>
       </c>
@@ -8375,7 +8387,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="128" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A128" s="2" t="s">
         <v>408</v>
       </c>
@@ -8398,7 +8410,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="129" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A129" s="2" t="s">
         <v>411</v>
       </c>
@@ -8421,7 +8433,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="130" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A130" s="2" t="s">
         <v>414</v>
       </c>
@@ -8444,7 +8456,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="131" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A131" s="2" t="s">
         <v>417</v>
       </c>
@@ -8467,7 +8479,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="132" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A132" s="2" t="s">
         <v>420</v>
       </c>
@@ -8490,7 +8502,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="133" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A133" s="2" t="s">
         <v>423</v>
       </c>
@@ -8513,7 +8525,7 @@
         <v>425</v>
       </c>
     </row>
-    <row r="134" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A134" s="2" t="s">
         <v>426</v>
       </c>
@@ -8536,7 +8548,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="135" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A135" s="2" t="s">
         <v>429</v>
       </c>
@@ -8559,7 +8571,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="136" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A136" s="2" t="s">
         <v>432</v>
       </c>
@@ -8582,7 +8594,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="137" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A137" s="2" t="s">
         <v>435</v>
       </c>
@@ -8605,7 +8617,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="138" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A138" s="2" t="s">
         <v>438</v>
       </c>
@@ -8628,7 +8640,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="139" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A139" s="2" t="s">
         <v>441</v>
       </c>
@@ -8651,7 +8663,7 @@
         <v>443</v>
       </c>
     </row>
-    <row r="140" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A140" s="2" t="s">
         <v>444</v>
       </c>
@@ -8674,7 +8686,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="141" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A141" s="2" t="s">
         <v>447</v>
       </c>
@@ -8697,7 +8709,7 @@
         <v>449</v>
       </c>
     </row>
-    <row r="142" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="142" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A142" s="2" t="s">
         <v>450</v>
       </c>
@@ -8720,7 +8732,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="143" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="143" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A143" s="2" t="s">
         <v>453</v>
       </c>
@@ -8743,7 +8755,7 @@
         <v>455</v>
       </c>
     </row>
-    <row r="144" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="144" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A144" s="2" t="s">
         <v>456</v>
       </c>
@@ -8766,7 +8778,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="145" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="145" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A145" s="2" t="s">
         <v>459</v>
       </c>
@@ -8789,7 +8801,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="146" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="146" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A146" s="2" t="s">
         <v>462</v>
       </c>
@@ -8812,7 +8824,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="147" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="147" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A147" s="2" t="s">
         <v>465</v>
       </c>
@@ -8835,7 +8847,7 @@
         <v>467</v>
       </c>
     </row>
-    <row r="148" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="148" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A148" s="2" t="s">
         <v>468</v>
       </c>
@@ -8858,7 +8870,7 @@
         <v>470</v>
       </c>
     </row>
-    <row r="149" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="149" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A149" s="2" t="s">
         <v>471</v>
       </c>
@@ -8881,7 +8893,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="150" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="150" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A150" s="2" t="s">
         <v>474</v>
       </c>
@@ -8904,7 +8916,7 @@
         <v>476</v>
       </c>
     </row>
-    <row r="151" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A151" s="2" t="s">
         <v>477</v>
       </c>
@@ -8927,7 +8939,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="152" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="152" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A152" s="2" t="s">
         <v>480</v>
       </c>
@@ -8950,7 +8962,7 @@
         <v>482</v>
       </c>
     </row>
-    <row r="153" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="153" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A153" s="2" t="s">
         <v>483</v>
       </c>
@@ -8973,7 +8985,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="154" spans="1:7" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="154" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A154" s="2" t="s">
         <v>486</v>
       </c>
@@ -8996,7 +9008,7 @@
         <v>488</v>
       </c>
     </row>
-    <row r="155" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="155" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A155" s="2" t="s">
         <v>489</v>
       </c>
@@ -9019,7 +9031,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="156" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="156" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A156" s="2" t="s">
         <v>492</v>
       </c>
@@ -9042,7 +9054,7 @@
         <v>494</v>
       </c>
     </row>
-    <row r="157" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="157" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A157" s="2" t="s">
         <v>495</v>
       </c>
@@ -9065,7 +9077,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="158" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="158" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A158" s="2" t="s">
         <v>498</v>
       </c>
@@ -9088,7 +9100,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="159" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="159" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A159" s="2" t="s">
         <v>501</v>
       </c>
@@ -9111,7 +9123,7 @@
         <v>503</v>
       </c>
     </row>
-    <row r="160" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="160" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A160" s="2" t="s">
         <v>504</v>
       </c>
@@ -9134,7 +9146,7 @@
         <v>506</v>
       </c>
     </row>
-    <row r="161" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="161" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A161" s="2" t="s">
         <v>507</v>
       </c>
@@ -9157,7 +9169,7 @@
         <v>509</v>
       </c>
     </row>
-    <row r="162" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="162" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A162" s="2" t="s">
         <v>510</v>
       </c>
@@ -9180,7 +9192,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="163" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="163" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A163" s="2" t="s">
         <v>513</v>
       </c>
@@ -9203,7 +9215,7 @@
         <v>515</v>
       </c>
     </row>
-    <row r="164" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="164" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A164" s="2" t="s">
         <v>516</v>
       </c>
@@ -9226,7 +9238,7 @@
         <v>518</v>
       </c>
     </row>
-    <row r="165" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="165" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A165" s="2" t="s">
         <v>519</v>
       </c>
@@ -9249,7 +9261,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="166" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="166" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A166" s="2" t="s">
         <v>522</v>
       </c>
@@ -9272,7 +9284,7 @@
         <v>524</v>
       </c>
     </row>
-    <row r="167" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="167" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A167" s="2" t="s">
         <v>525</v>
       </c>
@@ -9295,7 +9307,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="168" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="168" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A168" s="2" t="s">
         <v>528</v>
       </c>
@@ -9318,7 +9330,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="169" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="169" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A169" s="2" t="s">
         <v>531</v>
       </c>
@@ -9341,7 +9353,7 @@
         <v>533</v>
       </c>
     </row>
-    <row r="170" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="170" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A170" s="2" t="s">
         <v>534</v>
       </c>
@@ -9364,7 +9376,7 @@
         <v>536</v>
       </c>
     </row>
-    <row r="171" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="171" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A171" s="2" t="s">
         <v>537</v>
       </c>
@@ -9387,7 +9399,7 @@
         <v>539</v>
       </c>
     </row>
-    <row r="172" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="172" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A172" s="2" t="s">
         <v>540</v>
       </c>
@@ -9410,7 +9422,7 @@
         <v>542</v>
       </c>
     </row>
-    <row r="173" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="173" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A173" s="2" t="s">
         <v>543</v>
       </c>
@@ -9433,7 +9445,7 @@
         <v>545</v>
       </c>
     </row>
-    <row r="174" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="174" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A174" s="2" t="s">
         <v>546</v>
       </c>
@@ -9456,7 +9468,7 @@
         <v>548</v>
       </c>
     </row>
-    <row r="175" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="175" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A175" s="2" t="s">
         <v>549</v>
       </c>
@@ -9479,7 +9491,7 @@
         <v>551</v>
       </c>
     </row>
-    <row r="176" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="176" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A176" s="2" t="s">
         <v>552</v>
       </c>
@@ -9502,7 +9514,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="177" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="177" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A177" s="2" t="s">
         <v>555</v>
       </c>
@@ -9525,7 +9537,7 @@
         <v>557</v>
       </c>
     </row>
-    <row r="178" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="178" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A178" s="2" t="s">
         <v>558</v>
       </c>
@@ -9548,7 +9560,7 @@
         <v>560</v>
       </c>
     </row>
-    <row r="179" spans="1:7" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="179" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A179" s="2" t="s">
         <v>561</v>
       </c>
@@ -9571,7 +9583,7 @@
         <v>563</v>
       </c>
     </row>
-    <row r="180" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="180" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A180" s="2" t="s">
         <v>564</v>
       </c>
@@ -9594,7 +9606,7 @@
         <v>566</v>
       </c>
     </row>
-    <row r="181" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="181" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A181" s="2" t="s">
         <v>567</v>
       </c>
@@ -9617,7 +9629,7 @@
         <v>569</v>
       </c>
     </row>
-    <row r="182" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="182" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A182" s="2" t="s">
         <v>570</v>
       </c>
@@ -9640,7 +9652,7 @@
         <v>572</v>
       </c>
     </row>
-    <row r="183" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="183" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A183" s="2" t="s">
         <v>573</v>
       </c>
@@ -9663,7 +9675,7 @@
         <v>575</v>
       </c>
     </row>
-    <row r="184" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="184" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A184" s="2" t="s">
         <v>576</v>
       </c>
@@ -9686,7 +9698,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="185" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="185" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A185" s="2" t="s">
         <v>579</v>
       </c>
@@ -9709,7 +9721,7 @@
         <v>581</v>
       </c>
     </row>
-    <row r="186" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="186" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A186" s="2" t="s">
         <v>582</v>
       </c>
@@ -9732,7 +9744,7 @@
         <v>584</v>
       </c>
     </row>
-    <row r="187" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="187" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A187" s="2" t="s">
         <v>585</v>
       </c>
@@ -9755,7 +9767,7 @@
         <v>587</v>
       </c>
     </row>
-    <row r="188" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="188" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A188" s="2" t="s">
         <v>588</v>
       </c>
@@ -9778,7 +9790,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="189" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="189" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A189" s="2" t="s">
         <v>591</v>
       </c>
@@ -9801,7 +9813,7 @@
         <v>593</v>
       </c>
     </row>
-    <row r="190" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="190" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A190" s="2" t="s">
         <v>594</v>
       </c>
@@ -9824,7 +9836,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="191" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="191" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A191" s="2" t="s">
         <v>597</v>
       </c>
@@ -9847,7 +9859,7 @@
         <v>599</v>
       </c>
     </row>
-    <row r="192" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="192" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A192" s="2" t="s">
         <v>600</v>
       </c>
@@ -9870,7 +9882,7 @@
         <v>602</v>
       </c>
     </row>
-    <row r="193" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="193" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A193" s="2" t="s">
         <v>603</v>
       </c>
@@ -9893,7 +9905,7 @@
         <v>605</v>
       </c>
     </row>
-    <row r="194" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="194" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A194" s="2" t="s">
         <v>606</v>
       </c>
@@ -9916,7 +9928,7 @@
         <v>608</v>
       </c>
     </row>
-    <row r="195" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="195" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A195" s="2" t="s">
         <v>609</v>
       </c>
@@ -9939,7 +9951,7 @@
         <v>611</v>
       </c>
     </row>
-    <row r="196" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="196" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A196" s="2" t="s">
         <v>612</v>
       </c>
@@ -9962,7 +9974,7 @@
         <v>614</v>
       </c>
     </row>
-    <row r="197" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="197" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A197" s="2" t="s">
         <v>615</v>
       </c>
@@ -9985,7 +9997,7 @@
         <v>617</v>
       </c>
     </row>
-    <row r="198" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="198" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A198" s="2" t="s">
         <v>618</v>
       </c>
@@ -10008,7 +10020,7 @@
         <v>620</v>
       </c>
     </row>
-    <row r="199" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="199" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A199" s="2" t="s">
         <v>621</v>
       </c>
@@ -10031,7 +10043,7 @@
         <v>623</v>
       </c>
     </row>
-    <row r="200" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="200" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A200" s="2" t="s">
         <v>624</v>
       </c>
@@ -10054,7 +10066,7 @@
         <v>626</v>
       </c>
     </row>
-    <row r="201" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="201" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A201" s="2" t="s">
         <v>627</v>
       </c>
@@ -10077,7 +10089,7 @@
         <v>629</v>
       </c>
     </row>
-    <row r="202" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="202" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A202" s="2" t="s">
         <v>630</v>
       </c>
@@ -10100,7 +10112,7 @@
         <v>632</v>
       </c>
     </row>
-    <row r="203" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="203" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A203" s="2" t="s">
         <v>633</v>
       </c>
@@ -10123,7 +10135,7 @@
         <v>635</v>
       </c>
     </row>
-    <row r="204" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="204" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A204" s="2" t="s">
         <v>636</v>
       </c>
@@ -10146,7 +10158,7 @@
         <v>638</v>
       </c>
     </row>
-    <row r="205" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="205" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A205" s="2" t="s">
         <v>639</v>
       </c>
@@ -10169,7 +10181,7 @@
         <v>641</v>
       </c>
     </row>
-    <row r="206" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="206" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A206" s="2" t="s">
         <v>642</v>
       </c>
@@ -10192,7 +10204,7 @@
         <v>644</v>
       </c>
     </row>
-    <row r="207" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="207" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A207" s="2" t="s">
         <v>645</v>
       </c>
@@ -10215,7 +10227,7 @@
         <v>647</v>
       </c>
     </row>
-    <row r="208" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="208" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A208" s="2" t="s">
         <v>648</v>
       </c>
@@ -10238,7 +10250,7 @@
         <v>650</v>
       </c>
     </row>
-    <row r="209" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="209" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A209" s="2" t="s">
         <v>651</v>
       </c>
@@ -10261,7 +10273,7 @@
         <v>653</v>
       </c>
     </row>
-    <row r="210" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="210" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A210" s="2" t="s">
         <v>654</v>
       </c>
@@ -10284,7 +10296,7 @@
         <v>657</v>
       </c>
     </row>
-    <row r="211" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="211" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A211" s="2" t="s">
         <v>658</v>
       </c>
@@ -10307,7 +10319,7 @@
         <v>660</v>
       </c>
     </row>
-    <row r="212" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="212" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A212" s="2" t="s">
         <v>661</v>
       </c>
@@ -10330,7 +10342,7 @@
         <v>663</v>
       </c>
     </row>
-    <row r="213" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="213" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A213" s="2" t="s">
         <v>664</v>
       </c>
@@ -10353,7 +10365,7 @@
         <v>666</v>
       </c>
     </row>
-    <row r="214" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="214" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A214" s="2" t="s">
         <v>667</v>
       </c>
@@ -10376,7 +10388,7 @@
         <v>669</v>
       </c>
     </row>
-    <row r="215" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="215" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A215" s="2" t="s">
         <v>670</v>
       </c>
@@ -10399,7 +10411,7 @@
         <v>672</v>
       </c>
     </row>
-    <row r="216" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="216" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A216" s="2" t="s">
         <v>673</v>
       </c>
@@ -10422,7 +10434,7 @@
         <v>675</v>
       </c>
     </row>
-    <row r="217" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="217" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A217" s="2" t="s">
         <v>676</v>
       </c>
@@ -10445,7 +10457,7 @@
         <v>678</v>
       </c>
     </row>
-    <row r="218" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="218" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A218" s="2" t="s">
         <v>679</v>
       </c>
@@ -10468,7 +10480,7 @@
         <v>681</v>
       </c>
     </row>
-    <row r="219" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="219" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A219" s="2" t="s">
         <v>682</v>
       </c>
@@ -10491,7 +10503,7 @@
         <v>684</v>
       </c>
     </row>
-    <row r="220" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="220" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A220" s="2" t="s">
         <v>685</v>
       </c>
@@ -10514,7 +10526,7 @@
         <v>687</v>
       </c>
     </row>
-    <row r="221" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="221" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A221" s="2" t="s">
         <v>688</v>
       </c>
@@ -10537,7 +10549,7 @@
         <v>690</v>
       </c>
     </row>
-    <row r="222" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="222" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A222" s="2" t="s">
         <v>691</v>
       </c>
@@ -10560,7 +10572,7 @@
         <v>693</v>
       </c>
     </row>
-    <row r="223" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="223" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A223" s="2" t="s">
         <v>694</v>
       </c>
@@ -10583,7 +10595,7 @@
         <v>696</v>
       </c>
     </row>
-    <row r="224" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="224" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A224" s="2" t="s">
         <v>697</v>
       </c>
@@ -10606,7 +10618,7 @@
         <v>700</v>
       </c>
     </row>
-    <row r="225" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="225" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A225" s="2" t="s">
         <v>701</v>
       </c>
@@ -10629,7 +10641,7 @@
         <v>703</v>
       </c>
     </row>
-    <row r="226" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="226" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A226" s="2" t="s">
         <v>704</v>
       </c>
@@ -10652,7 +10664,7 @@
         <v>706</v>
       </c>
     </row>
-    <row r="227" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="227" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A227" s="2" t="s">
         <v>707</v>
       </c>
@@ -10675,7 +10687,7 @@
         <v>709</v>
       </c>
     </row>
-    <row r="228" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="228" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A228" s="2" t="s">
         <v>710</v>
       </c>
@@ -10698,7 +10710,7 @@
         <v>713</v>
       </c>
     </row>
-    <row r="229" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="229" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A229" s="2" t="s">
         <v>714</v>
       </c>
@@ -10721,7 +10733,7 @@
         <v>716</v>
       </c>
     </row>
-    <row r="230" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="230" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A230" s="2" t="s">
         <v>717</v>
       </c>
@@ -10744,7 +10756,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="231" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="231" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A231" s="2" t="s">
         <v>720</v>
       </c>
@@ -10767,7 +10779,7 @@
         <v>722</v>
       </c>
     </row>
-    <row r="232" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="232" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A232" s="2" t="s">
         <v>723</v>
       </c>
@@ -10790,7 +10802,7 @@
         <v>725</v>
       </c>
     </row>
-    <row r="233" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="233" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A233" s="2" t="s">
         <v>726</v>
       </c>
@@ -10813,7 +10825,7 @@
         <v>729</v>
       </c>
     </row>
-    <row r="234" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="234" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A234" s="2" t="s">
         <v>730</v>
       </c>
@@ -10836,7 +10848,7 @@
         <v>732</v>
       </c>
     </row>
-    <row r="235" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="235" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A235" s="2" t="s">
         <v>733</v>
       </c>
@@ -10859,7 +10871,7 @@
         <v>735</v>
       </c>
     </row>
-    <row r="236" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="236" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A236" s="2" t="s">
         <v>736</v>
       </c>
@@ -10882,7 +10894,7 @@
         <v>738</v>
       </c>
     </row>
-    <row r="237" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="237" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A237" s="2" t="s">
         <v>739</v>
       </c>
@@ -10905,7 +10917,7 @@
         <v>741</v>
       </c>
     </row>
-    <row r="238" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="238" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A238" s="2" t="s">
         <v>742</v>
       </c>
@@ -10928,7 +10940,7 @@
         <v>744</v>
       </c>
     </row>
-    <row r="239" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="239" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A239" s="2" t="s">
         <v>745</v>
       </c>
@@ -10951,7 +10963,7 @@
         <v>747</v>
       </c>
     </row>
-    <row r="240" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="240" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A240" s="2" t="s">
         <v>748</v>
       </c>
@@ -10974,7 +10986,7 @@
         <v>750</v>
       </c>
     </row>
-    <row r="241" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="241" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A241" s="2" t="s">
         <v>751</v>
       </c>
@@ -10997,7 +11009,7 @@
         <v>753</v>
       </c>
     </row>
-    <row r="242" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="242" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A242" s="2" t="s">
         <v>754</v>
       </c>
@@ -11020,7 +11032,7 @@
         <v>756</v>
       </c>
     </row>
-    <row r="243" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="243" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A243" s="2" t="s">
         <v>757</v>
       </c>
@@ -11043,7 +11055,7 @@
         <v>759</v>
       </c>
     </row>
-    <row r="244" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="244" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A244" s="2" t="s">
         <v>760</v>
       </c>
@@ -11066,7 +11078,7 @@
         <v>762</v>
       </c>
     </row>
-    <row r="245" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="245" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A245" s="2" t="s">
         <v>763</v>
       </c>
@@ -11089,7 +11101,7 @@
         <v>765</v>
       </c>
     </row>
-    <row r="246" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="246" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A246" s="2" t="s">
         <v>766</v>
       </c>
@@ -11112,7 +11124,7 @@
         <v>768</v>
       </c>
     </row>
-    <row r="247" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="247" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A247" s="2" t="s">
         <v>769</v>
       </c>
@@ -11135,7 +11147,7 @@
         <v>771</v>
       </c>
     </row>
-    <row r="248" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="248" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A248" s="2" t="s">
         <v>772</v>
       </c>
@@ -11158,7 +11170,7 @@
         <v>774</v>
       </c>
     </row>
-    <row r="249" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="249" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A249" s="2" t="s">
         <v>775</v>
       </c>
@@ -11181,7 +11193,7 @@
         <v>777</v>
       </c>
     </row>
-    <row r="250" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="250" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A250" s="2" t="s">
         <v>778</v>
       </c>
@@ -11204,7 +11216,7 @@
         <v>780</v>
       </c>
     </row>
-    <row r="251" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="251" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A251" s="2" t="s">
         <v>781</v>
       </c>
@@ -11227,7 +11239,7 @@
         <v>783</v>
       </c>
     </row>
-    <row r="252" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="252" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A252" s="2" t="s">
         <v>784</v>
       </c>
@@ -11250,7 +11262,7 @@
         <v>786</v>
       </c>
     </row>
-    <row r="253" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="253" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A253" s="2" t="s">
         <v>787</v>
       </c>
@@ -11273,7 +11285,7 @@
         <v>789</v>
       </c>
     </row>
-    <row r="254" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="254" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A254" s="2" t="s">
         <v>790</v>
       </c>
@@ -11296,7 +11308,7 @@
         <v>792</v>
       </c>
     </row>
-    <row r="255" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="255" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A255" s="2" t="s">
         <v>793</v>
       </c>
@@ -11319,7 +11331,7 @@
         <v>795</v>
       </c>
     </row>
-    <row r="256" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="256" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A256" s="2" t="s">
         <v>796</v>
       </c>
@@ -11342,7 +11354,7 @@
         <v>798</v>
       </c>
     </row>
-    <row r="257" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="257" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A257" s="2" t="s">
         <v>799</v>
       </c>
@@ -11365,7 +11377,7 @@
         <v>801</v>
       </c>
     </row>
-    <row r="258" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="258" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A258" s="2" t="s">
         <v>802</v>
       </c>
@@ -11388,7 +11400,7 @@
         <v>804</v>
       </c>
     </row>
-    <row r="259" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="259" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A259" s="2" t="s">
         <v>805</v>
       </c>
@@ -11411,7 +11423,7 @@
         <v>807</v>
       </c>
     </row>
-    <row r="260" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="260" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A260" s="2" t="s">
         <v>808</v>
       </c>
@@ -11434,7 +11446,7 @@
         <v>810</v>
       </c>
     </row>
-    <row r="261" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="261" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A261" s="2" t="s">
         <v>811</v>
       </c>
@@ -11457,7 +11469,7 @@
         <v>813</v>
       </c>
     </row>
-    <row r="262" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="262" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A262" s="2" t="s">
         <v>814</v>
       </c>
@@ -11480,7 +11492,7 @@
         <v>816</v>
       </c>
     </row>
-    <row r="263" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="263" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A263" s="2" t="s">
         <v>817</v>
       </c>
@@ -11503,7 +11515,7 @@
         <v>819</v>
       </c>
     </row>
-    <row r="264" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="264" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A264" s="2" t="s">
         <v>820</v>
       </c>
@@ -11526,7 +11538,7 @@
         <v>822</v>
       </c>
     </row>
-    <row r="265" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="265" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A265" s="2" t="s">
         <v>823</v>
       </c>
@@ -11549,7 +11561,7 @@
         <v>825</v>
       </c>
     </row>
-    <row r="266" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="266" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A266" s="2" t="s">
         <v>826</v>
       </c>
@@ -11572,7 +11584,7 @@
         <v>828</v>
       </c>
     </row>
-    <row r="267" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="267" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A267" s="2" t="s">
         <v>829</v>
       </c>
@@ -11595,7 +11607,7 @@
         <v>831</v>
       </c>
     </row>
-    <row r="268" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="268" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A268" s="2" t="s">
         <v>832</v>
       </c>
@@ -11618,7 +11630,7 @@
         <v>834</v>
       </c>
     </row>
-    <row r="269" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="269" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A269" s="2" t="s">
         <v>835</v>
       </c>
@@ -11641,7 +11653,7 @@
         <v>837</v>
       </c>
     </row>
-    <row r="270" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="270" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A270" s="2" t="s">
         <v>838</v>
       </c>
@@ -11664,7 +11676,7 @@
         <v>840</v>
       </c>
     </row>
-    <row r="271" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="271" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A271" s="2" t="s">
         <v>841</v>
       </c>
@@ -11687,7 +11699,7 @@
         <v>844</v>
       </c>
     </row>
-    <row r="272" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="272" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A272" s="2" t="s">
         <v>845</v>
       </c>
@@ -11710,7 +11722,7 @@
         <v>847</v>
       </c>
     </row>
-    <row r="273" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="273" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A273" s="2" t="s">
         <v>848</v>
       </c>
@@ -11733,7 +11745,7 @@
         <v>850</v>
       </c>
     </row>
-    <row r="274" spans="1:7" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="274" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A274" s="2" t="s">
         <v>851</v>
       </c>
@@ -11756,7 +11768,7 @@
         <v>853</v>
       </c>
     </row>
-    <row r="275" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="275" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A275" s="2" t="s">
         <v>854</v>
       </c>
@@ -11779,7 +11791,7 @@
         <v>856</v>
       </c>
     </row>
-    <row r="276" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="276" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A276" s="2" t="s">
         <v>857</v>
       </c>
@@ -11802,7 +11814,7 @@
         <v>859</v>
       </c>
     </row>
-    <row r="277" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="277" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A277" s="2" t="s">
         <v>860</v>
       </c>
@@ -11825,7 +11837,7 @@
         <v>862</v>
       </c>
     </row>
-    <row r="278" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="278" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A278" s="2" t="s">
         <v>863</v>
       </c>
@@ -11848,7 +11860,7 @@
         <v>865</v>
       </c>
     </row>
-    <row r="279" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="279" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A279" s="2" t="s">
         <v>866</v>
       </c>
@@ -11871,7 +11883,7 @@
         <v>868</v>
       </c>
     </row>
-    <row r="280" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="280" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A280" s="2" t="s">
         <v>869</v>
       </c>
@@ -11894,7 +11906,7 @@
         <v>871</v>
       </c>
     </row>
-    <row r="281" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="281" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A281" s="2" t="s">
         <v>872</v>
       </c>
@@ -11917,7 +11929,7 @@
         <v>874</v>
       </c>
     </row>
-    <row r="282" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="282" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A282" s="2" t="s">
         <v>875</v>
       </c>
@@ -11940,7 +11952,7 @@
         <v>878</v>
       </c>
     </row>
-    <row r="283" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="283" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A283" s="2" t="s">
         <v>879</v>
       </c>
@@ -11963,7 +11975,7 @@
         <v>881</v>
       </c>
     </row>
-    <row r="284" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="284" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A284" s="2" t="s">
         <v>882</v>
       </c>
@@ -11986,7 +11998,7 @@
         <v>884</v>
       </c>
     </row>
-    <row r="285" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="285" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A285" s="2" t="s">
         <v>885</v>
       </c>
@@ -12009,7 +12021,7 @@
         <v>887</v>
       </c>
     </row>
-    <row r="286" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="286" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A286" s="2" t="s">
         <v>888</v>
       </c>
@@ -12032,7 +12044,7 @@
         <v>890</v>
       </c>
     </row>
-    <row r="287" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="287" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A287" s="2" t="s">
         <v>891</v>
       </c>
@@ -12055,7 +12067,7 @@
         <v>893</v>
       </c>
     </row>
-    <row r="288" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="288" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A288" s="2" t="s">
         <v>894</v>
       </c>
@@ -12078,7 +12090,7 @@
         <v>896</v>
       </c>
     </row>
-    <row r="289" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="289" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A289" s="2" t="s">
         <v>897</v>
       </c>
@@ -12101,7 +12113,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="290" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="290" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A290" s="2" t="s">
         <v>900</v>
       </c>
@@ -12124,7 +12136,7 @@
         <v>902</v>
       </c>
     </row>
-    <row r="291" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="291" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A291" s="2" t="s">
         <v>903</v>
       </c>
@@ -12147,7 +12159,7 @@
         <v>905</v>
       </c>
     </row>
-    <row r="292" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="292" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A292" s="2" t="s">
         <v>906</v>
       </c>
@@ -12170,7 +12182,7 @@
         <v>908</v>
       </c>
     </row>
-    <row r="293" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="293" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A293" s="2" t="s">
         <v>909</v>
       </c>
@@ -12193,7 +12205,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="294" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="294" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A294" s="2" t="s">
         <v>912</v>
       </c>
@@ -12216,7 +12228,7 @@
         <v>914</v>
       </c>
     </row>
-    <row r="295" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="295" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A295" s="2" t="s">
         <v>915</v>
       </c>
@@ -12239,7 +12251,7 @@
         <v>917</v>
       </c>
     </row>
-    <row r="296" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="296" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A296" s="2" t="s">
         <v>918</v>
       </c>
@@ -12262,7 +12274,7 @@
         <v>920</v>
       </c>
     </row>
-    <row r="297" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="297" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A297" s="2" t="s">
         <v>921</v>
       </c>
@@ -12285,7 +12297,7 @@
         <v>923</v>
       </c>
     </row>
-    <row r="298" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="298" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A298" s="2" t="s">
         <v>924</v>
       </c>
@@ -12308,7 +12320,7 @@
         <v>926</v>
       </c>
     </row>
-    <row r="299" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="299" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A299" s="2" t="s">
         <v>927</v>
       </c>
@@ -12331,7 +12343,7 @@
         <v>929</v>
       </c>
     </row>
-    <row r="300" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="300" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A300" s="2" t="s">
         <v>930</v>
       </c>
@@ -12354,7 +12366,7 @@
         <v>932</v>
       </c>
     </row>
-    <row r="301" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="301" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A301" s="2" t="s">
         <v>933</v>
       </c>
@@ -12377,7 +12389,7 @@
         <v>935</v>
       </c>
     </row>
-    <row r="302" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="302" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A302" s="2" t="s">
         <v>936</v>
       </c>
@@ -12400,7 +12412,7 @@
         <v>938</v>
       </c>
     </row>
-    <row r="303" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="303" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A303" s="2" t="s">
         <v>939</v>
       </c>
@@ -12423,7 +12435,7 @@
         <v>941</v>
       </c>
     </row>
-    <row r="304" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="304" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A304" s="2" t="s">
         <v>942</v>
       </c>
@@ -12446,7 +12458,7 @@
         <v>944</v>
       </c>
     </row>
-    <row r="305" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="305" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A305" s="2" t="s">
         <v>945</v>
       </c>
@@ -12469,7 +12481,7 @@
         <v>947</v>
       </c>
     </row>
-    <row r="306" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="306" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A306" s="2" t="s">
         <v>948</v>
       </c>
@@ -12492,7 +12504,7 @@
         <v>950</v>
       </c>
     </row>
-    <row r="307" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="307" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A307" s="2" t="s">
         <v>951</v>
       </c>
@@ -12515,7 +12527,7 @@
         <v>953</v>
       </c>
     </row>
-    <row r="308" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="308" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A308" s="2" t="s">
         <v>954</v>
       </c>
@@ -12538,7 +12550,7 @@
         <v>956</v>
       </c>
     </row>
-    <row r="309" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="309" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A309" s="2" t="s">
         <v>957</v>
       </c>
@@ -12561,7 +12573,7 @@
         <v>959</v>
       </c>
     </row>
-    <row r="310" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="310" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A310" s="2" t="s">
         <v>960</v>
       </c>
@@ -12584,7 +12596,7 @@
         <v>962</v>
       </c>
     </row>
-    <row r="311" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="311" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A311" s="2" t="s">
         <v>963</v>
       </c>
@@ -12607,7 +12619,7 @@
         <v>965</v>
       </c>
     </row>
-    <row r="312" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="312" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A312" s="2" t="s">
         <v>966</v>
       </c>
@@ -12630,7 +12642,7 @@
         <v>968</v>
       </c>
     </row>
-    <row r="313" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="313" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A313" s="2" t="s">
         <v>969</v>
       </c>
@@ -12653,7 +12665,7 @@
         <v>971</v>
       </c>
     </row>
-    <row r="314" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="314" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A314" s="2" t="s">
         <v>972</v>
       </c>
@@ -12676,7 +12688,7 @@
         <v>974</v>
       </c>
     </row>
-    <row r="315" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="315" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A315" s="2" t="s">
         <v>975</v>
       </c>
@@ -12699,7 +12711,7 @@
         <v>977</v>
       </c>
     </row>
-    <row r="316" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="316" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A316" s="2" t="s">
         <v>978</v>
       </c>
@@ -12722,7 +12734,7 @@
         <v>980</v>
       </c>
     </row>
-    <row r="317" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="317" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A317" s="2" t="s">
         <v>981</v>
       </c>
@@ -12745,7 +12757,7 @@
         <v>983</v>
       </c>
     </row>
-    <row r="318" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="318" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A318" s="2" t="s">
         <v>984</v>
       </c>
@@ -12768,7 +12780,7 @@
         <v>986</v>
       </c>
     </row>
-    <row r="319" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="319" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A319" s="2" t="s">
         <v>987</v>
       </c>
@@ -12791,7 +12803,7 @@
         <v>989</v>
       </c>
     </row>
-    <row r="320" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="320" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A320" s="2" t="s">
         <v>990</v>
       </c>
@@ -12814,7 +12826,7 @@
         <v>992</v>
       </c>
     </row>
-    <row r="321" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="321" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A321" s="2" t="s">
         <v>993</v>
       </c>
@@ -12837,7 +12849,7 @@
         <v>995</v>
       </c>
     </row>
-    <row r="322" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="322" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A322" s="2" t="s">
         <v>996</v>
       </c>
@@ -12860,7 +12872,7 @@
         <v>998</v>
       </c>
     </row>
-    <row r="323" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="323" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A323" s="2" t="s">
         <v>999</v>
       </c>
@@ -12883,7 +12895,7 @@
         <v>1001</v>
       </c>
     </row>
-    <row r="324" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="324" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A324" s="2" t="s">
         <v>1002</v>
       </c>
@@ -12906,7 +12918,7 @@
         <v>1004</v>
       </c>
     </row>
-    <row r="325" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="325" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A325" s="2" t="s">
         <v>1005</v>
       </c>
@@ -12929,7 +12941,7 @@
         <v>1007</v>
       </c>
     </row>
-    <row r="326" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="326" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A326" s="2" t="s">
         <v>1008</v>
       </c>
@@ -12952,7 +12964,7 @@
         <v>1010</v>
       </c>
     </row>
-    <row r="327" spans="1:7" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="327" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A327" s="2" t="s">
         <v>1011</v>
       </c>
@@ -12975,7 +12987,7 @@
         <v>1013</v>
       </c>
     </row>
-    <row r="328" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="328" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A328" s="2" t="s">
         <v>1014</v>
       </c>
@@ -12998,7 +13010,7 @@
         <v>1016</v>
       </c>
     </row>
-    <row r="329" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="329" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A329" s="2" t="s">
         <v>1017</v>
       </c>
@@ -13021,7 +13033,7 @@
         <v>1020</v>
       </c>
     </row>
-    <row r="330" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="330" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A330" s="2" t="s">
         <v>1021</v>
       </c>
@@ -13044,7 +13056,7 @@
         <v>1023</v>
       </c>
     </row>
-    <row r="331" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="331" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A331" s="2" t="s">
         <v>1024</v>
       </c>
@@ -13067,7 +13079,7 @@
         <v>1026</v>
       </c>
     </row>
-    <row r="332" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="332" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A332" s="2" t="s">
         <v>1027</v>
       </c>
@@ -13090,7 +13102,7 @@
         <v>1029</v>
       </c>
     </row>
-    <row r="333" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="333" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A333" s="2" t="s">
         <v>1030</v>
       </c>
@@ -13113,7 +13125,7 @@
         <v>1032</v>
       </c>
     </row>
-    <row r="334" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="334" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A334" s="2" t="s">
         <v>1033</v>
       </c>
@@ -13136,7 +13148,7 @@
         <v>1035</v>
       </c>
     </row>
-    <row r="335" spans="1:7" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="335" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A335" s="2" t="s">
         <v>1036</v>
       </c>
@@ -13159,7 +13171,7 @@
         <v>1038</v>
       </c>
     </row>
-    <row r="336" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="336" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A336" s="2" t="s">
         <v>1039</v>
       </c>
@@ -13182,7 +13194,7 @@
         <v>1041</v>
       </c>
     </row>
-    <row r="337" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="337" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A337" s="2" t="s">
         <v>1042</v>
       </c>
@@ -13205,7 +13217,7 @@
         <v>1044</v>
       </c>
     </row>
-    <row r="338" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="338" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A338" s="2" t="s">
         <v>1045</v>
       </c>
@@ -13228,7 +13240,7 @@
         <v>1048</v>
       </c>
     </row>
-    <row r="339" spans="1:7" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="339" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A339" s="2" t="s">
         <v>1049</v>
       </c>
@@ -13251,7 +13263,7 @@
         <v>1051</v>
       </c>
     </row>
-    <row r="340" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="340" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A340" s="2" t="s">
         <v>1052</v>
       </c>
@@ -13274,7 +13286,7 @@
         <v>1054</v>
       </c>
     </row>
-    <row r="341" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="341" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A341" s="2" t="s">
         <v>1055</v>
       </c>
@@ -13297,7 +13309,7 @@
         <v>1057</v>
       </c>
     </row>
-    <row r="342" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="342" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A342" s="2" t="s">
         <v>1058</v>
       </c>
@@ -13320,7 +13332,7 @@
         <v>1060</v>
       </c>
     </row>
-    <row r="343" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="343" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A343" s="2" t="s">
         <v>1061</v>
       </c>
@@ -13343,7 +13355,7 @@
         <v>1063</v>
       </c>
     </row>
-    <row r="344" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="344" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A344" s="2" t="s">
         <v>1064</v>
       </c>
@@ -13366,7 +13378,7 @@
         <v>1066</v>
       </c>
     </row>
-    <row r="345" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="345" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A345" s="2" t="s">
         <v>1067</v>
       </c>
@@ -13389,7 +13401,7 @@
         <v>1069</v>
       </c>
     </row>
-    <row r="346" spans="1:7" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="346" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A346" s="2" t="s">
         <v>1070</v>
       </c>
@@ -13412,7 +13424,7 @@
         <v>1072</v>
       </c>
     </row>
-    <row r="347" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="347" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A347" s="2" t="s">
         <v>1073</v>
       </c>
@@ -13435,7 +13447,7 @@
         <v>1075</v>
       </c>
     </row>
-    <row r="348" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="348" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A348" s="2" t="s">
         <v>1076</v>
       </c>
@@ -13458,7 +13470,7 @@
         <v>1078</v>
       </c>
     </row>
-    <row r="349" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="349" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A349" s="2" t="s">
         <v>1079</v>
       </c>
@@ -13481,7 +13493,7 @@
         <v>1081</v>
       </c>
     </row>
-    <row r="350" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="350" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A350" s="2" t="s">
         <v>1082</v>
       </c>
@@ -13504,7 +13516,7 @@
         <v>1084</v>
       </c>
     </row>
-    <row r="351" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="351" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A351" s="2" t="s">
         <v>1085</v>
       </c>
@@ -13527,7 +13539,7 @@
         <v>1087</v>
       </c>
     </row>
-    <row r="352" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="352" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A352" s="2" t="s">
         <v>1088</v>
       </c>
@@ -13550,7 +13562,7 @@
         <v>1090</v>
       </c>
     </row>
-    <row r="353" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="353" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A353" s="2" t="s">
         <v>1091</v>
       </c>
@@ -13573,7 +13585,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="354" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="354" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A354" s="2" t="s">
         <v>1094</v>
       </c>
@@ -13596,7 +13608,7 @@
         <v>1096</v>
       </c>
     </row>
-    <row r="355" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="355" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A355" s="2" t="s">
         <v>1097</v>
       </c>
@@ -13619,7 +13631,7 @@
         <v>1099</v>
       </c>
     </row>
-    <row r="356" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="356" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A356" s="2" t="s">
         <v>1100</v>
       </c>
@@ -13642,7 +13654,7 @@
         <v>1102</v>
       </c>
     </row>
-    <row r="357" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="357" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A357" s="2" t="s">
         <v>1103</v>
       </c>
@@ -13665,7 +13677,7 @@
         <v>1105</v>
       </c>
     </row>
-    <row r="358" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="358" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A358" s="2" t="s">
         <v>1106</v>
       </c>
@@ -13688,7 +13700,7 @@
         <v>1108</v>
       </c>
     </row>
-    <row r="359" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="359" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A359" s="2" t="s">
         <v>1109</v>
       </c>
@@ -13711,7 +13723,7 @@
         <v>1111</v>
       </c>
     </row>
-    <row r="360" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="360" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A360" s="2" t="s">
         <v>1112</v>
       </c>
@@ -13734,7 +13746,7 @@
         <v>1115</v>
       </c>
     </row>
-    <row r="361" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="361" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A361" s="2" t="s">
         <v>1116</v>
       </c>
@@ -13757,7 +13769,7 @@
         <v>1118</v>
       </c>
     </row>
-    <row r="362" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="362" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A362" s="2" t="s">
         <v>1119</v>
       </c>
@@ -13780,7 +13792,7 @@
         <v>1121</v>
       </c>
     </row>
-    <row r="363" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="363" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A363" s="2" t="s">
         <v>1122</v>
       </c>
@@ -13803,7 +13815,7 @@
         <v>1124</v>
       </c>
     </row>
-    <row r="364" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="364" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A364" s="2" t="s">
         <v>1125</v>
       </c>
@@ -13826,7 +13838,7 @@
         <v>1127</v>
       </c>
     </row>
-    <row r="365" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="365" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A365" s="2" t="s">
         <v>1128</v>
       </c>
@@ -13849,7 +13861,7 @@
         <v>1130</v>
       </c>
     </row>
-    <row r="366" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="366" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A366" s="2" t="s">
         <v>1131</v>
       </c>
@@ -13872,7 +13884,7 @@
         <v>1133</v>
       </c>
     </row>
-    <row r="367" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="367" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A367" s="2" t="s">
         <v>1134</v>
       </c>
@@ -13895,7 +13907,7 @@
         <v>1136</v>
       </c>
     </row>
-    <row r="368" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="368" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A368" s="2" t="s">
         <v>1137</v>
       </c>
@@ -13918,7 +13930,7 @@
         <v>1139</v>
       </c>
     </row>
-    <row r="369" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="369" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A369" s="2" t="s">
         <v>1140</v>
       </c>
@@ -13941,7 +13953,7 @@
         <v>1142</v>
       </c>
     </row>
-    <row r="370" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="370" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A370" s="2" t="s">
         <v>1143</v>
       </c>
@@ -13964,7 +13976,7 @@
         <v>1145</v>
       </c>
     </row>
-    <row r="371" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="371" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A371" s="2" t="s">
         <v>1146</v>
       </c>
@@ -13987,7 +13999,7 @@
         <v>1148</v>
       </c>
     </row>
-    <row r="372" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="372" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A372" s="2" t="s">
         <v>1149</v>
       </c>
@@ -14010,7 +14022,7 @@
         <v>1151</v>
       </c>
     </row>
-    <row r="373" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="373" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A373" s="2" t="s">
         <v>1152</v>
       </c>
@@ -14033,7 +14045,7 @@
         <v>1154</v>
       </c>
     </row>
-    <row r="374" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="374" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A374" s="2" t="s">
         <v>1155</v>
       </c>
@@ -14056,7 +14068,7 @@
         <v>1157</v>
       </c>
     </row>
-    <row r="375" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="375" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A375" s="2" t="s">
         <v>1158</v>
       </c>
@@ -14079,7 +14091,7 @@
         <v>1160</v>
       </c>
     </row>
-    <row r="376" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="376" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A376" s="2" t="s">
         <v>1161</v>
       </c>
@@ -14102,7 +14114,7 @@
         <v>1163</v>
       </c>
     </row>
-    <row r="377" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="377" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A377" s="2" t="s">
         <v>1164</v>
       </c>
@@ -14125,7 +14137,7 @@
         <v>1166</v>
       </c>
     </row>
-    <row r="378" spans="1:7" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="378" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A378" s="2" t="s">
         <v>1167</v>
       </c>
@@ -14148,7 +14160,7 @@
         <v>1169</v>
       </c>
     </row>
-    <row r="379" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="379" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A379" s="2" t="s">
         <v>1170</v>
       </c>
@@ -14171,7 +14183,7 @@
         <v>1172</v>
       </c>
     </row>
-    <row r="380" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="380" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A380" s="2" t="s">
         <v>1173</v>
       </c>
@@ -14194,7 +14206,7 @@
         <v>1175</v>
       </c>
     </row>
-    <row r="381" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="381" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A381" s="2" t="s">
         <v>1176</v>
       </c>
@@ -14217,7 +14229,7 @@
         <v>1178</v>
       </c>
     </row>
-    <row r="382" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="382" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A382" s="2" t="s">
         <v>1179</v>
       </c>
@@ -14240,7 +14252,7 @@
         <v>1181</v>
       </c>
     </row>
-    <row r="383" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="383" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A383" s="2" t="s">
         <v>1182</v>
       </c>
@@ -14263,7 +14275,7 @@
         <v>1184</v>
       </c>
     </row>
-    <row r="384" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="384" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A384" s="2" t="s">
         <v>1185</v>
       </c>
@@ -14286,7 +14298,7 @@
         <v>1187</v>
       </c>
     </row>
-    <row r="385" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="385" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A385" s="2" t="s">
         <v>1188</v>
       </c>
@@ -14309,7 +14321,7 @@
         <v>1190</v>
       </c>
     </row>
-    <row r="386" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="386" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A386" s="2" t="s">
         <v>1191</v>
       </c>
@@ -14332,7 +14344,7 @@
         <v>1193</v>
       </c>
     </row>
-    <row r="387" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="387" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A387" s="2" t="s">
         <v>1194</v>
       </c>
@@ -14355,7 +14367,7 @@
         <v>1196</v>
       </c>
     </row>
-    <row r="388" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="388" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A388" s="2" t="s">
         <v>1197</v>
       </c>
@@ -14378,7 +14390,7 @@
         <v>1199</v>
       </c>
     </row>
-    <row r="389" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="389" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A389" s="2" t="s">
         <v>1200</v>
       </c>
@@ -14401,7 +14413,7 @@
         <v>1202</v>
       </c>
     </row>
-    <row r="390" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="390" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A390" s="2" t="s">
         <v>1203</v>
       </c>
@@ -14424,7 +14436,7 @@
         <v>1205</v>
       </c>
     </row>
-    <row r="391" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="391" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A391" s="2" t="s">
         <v>1206</v>
       </c>
@@ -14447,7 +14459,7 @@
         <v>1208</v>
       </c>
     </row>
-    <row r="392" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="392" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A392" s="2" t="s">
         <v>1209</v>
       </c>
@@ -14470,7 +14482,7 @@
         <v>1211</v>
       </c>
     </row>
-    <row r="393" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="393" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A393" s="2" t="s">
         <v>1212</v>
       </c>
@@ -14493,7 +14505,7 @@
         <v>1214</v>
       </c>
     </row>
-    <row r="394" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="394" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A394" s="2" t="s">
         <v>1215</v>
       </c>
@@ -14516,7 +14528,7 @@
         <v>1217</v>
       </c>
     </row>
-    <row r="395" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="395" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A395" s="2" t="s">
         <v>1218</v>
       </c>
@@ -14539,7 +14551,7 @@
         <v>1220</v>
       </c>
     </row>
-    <row r="396" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="396" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A396" s="2" t="s">
         <v>1221</v>
       </c>
@@ -14562,7 +14574,7 @@
         <v>1223</v>
       </c>
     </row>
-    <row r="397" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="397" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A397" s="2" t="s">
         <v>1224</v>
       </c>
@@ -14585,7 +14597,7 @@
         <v>1226</v>
       </c>
     </row>
-    <row r="398" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="398" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A398" s="2" t="s">
         <v>1227</v>
       </c>
@@ -14608,7 +14620,7 @@
         <v>1229</v>
       </c>
     </row>
-    <row r="399" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="399" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A399" s="2" t="s">
         <v>1230</v>
       </c>
@@ -14631,7 +14643,7 @@
         <v>1232</v>
       </c>
     </row>
-    <row r="400" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="400" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A400" s="2" t="s">
         <v>1233</v>
       </c>
@@ -14654,7 +14666,7 @@
         <v>1235</v>
       </c>
     </row>
-    <row r="401" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="401" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A401" s="2" t="s">
         <v>1236</v>
       </c>
@@ -14677,7 +14689,7 @@
         <v>1238</v>
       </c>
     </row>
-    <row r="402" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="402" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A402" s="2" t="s">
         <v>1239</v>
       </c>
@@ -14700,7 +14712,7 @@
         <v>1241</v>
       </c>
     </row>
-    <row r="403" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="403" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A403" s="2" t="s">
         <v>1242</v>
       </c>
@@ -14723,7 +14735,7 @@
         <v>1244</v>
       </c>
     </row>
-    <row r="404" spans="1:7" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="404" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A404" s="2" t="s">
         <v>1245</v>
       </c>
@@ -14746,7 +14758,7 @@
         <v>1247</v>
       </c>
     </row>
-    <row r="405" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="405" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A405" s="2" t="s">
         <v>1248</v>
       </c>
@@ -14769,7 +14781,7 @@
         <v>1250</v>
       </c>
     </row>
-    <row r="406" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="406" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A406" s="2" t="s">
         <v>1251</v>
       </c>
@@ -14792,7 +14804,7 @@
         <v>1253</v>
       </c>
     </row>
-    <row r="407" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="407" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A407" s="2" t="s">
         <v>1254</v>
       </c>
@@ -14815,7 +14827,7 @@
         <v>1256</v>
       </c>
     </row>
-    <row r="408" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="408" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A408" s="2" t="s">
         <v>1257</v>
       </c>
@@ -14838,7 +14850,7 @@
         <v>1259</v>
       </c>
     </row>
-    <row r="409" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="409" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A409" s="2" t="s">
         <v>1260</v>
       </c>
@@ -14861,7 +14873,7 @@
         <v>1262</v>
       </c>
     </row>
-    <row r="410" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="410" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A410" s="2" t="s">
         <v>1263</v>
       </c>
@@ -14884,7 +14896,7 @@
         <v>1265</v>
       </c>
     </row>
-    <row r="411" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="411" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A411" s="2" t="s">
         <v>1266</v>
       </c>
@@ -14907,7 +14919,7 @@
         <v>1268</v>
       </c>
     </row>
-    <row r="412" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="412" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A412" s="2" t="s">
         <v>1269</v>
       </c>
@@ -14930,7 +14942,7 @@
         <v>1271</v>
       </c>
     </row>
-    <row r="413" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="413" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A413" s="2" t="s">
         <v>1272</v>
       </c>
@@ -14953,7 +14965,7 @@
         <v>1274</v>
       </c>
     </row>
-    <row r="414" spans="1:7" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="414" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A414" s="2" t="s">
         <v>1275</v>
       </c>
@@ -14976,7 +14988,7 @@
         <v>1277</v>
       </c>
     </row>
-    <row r="415" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="415" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A415" s="2" t="s">
         <v>1278</v>
       </c>
@@ -14999,7 +15011,7 @@
         <v>1281</v>
       </c>
     </row>
-    <row r="416" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="416" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A416" s="2" t="s">
         <v>1282</v>
       </c>
@@ -15022,7 +15034,7 @@
         <v>1284</v>
       </c>
     </row>
-    <row r="417" spans="1:7" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="417" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A417" s="2" t="s">
         <v>1285</v>
       </c>
@@ -15045,7 +15057,7 @@
         <v>1288</v>
       </c>
     </row>
-    <row r="418" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="418" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A418" s="2" t="s">
         <v>1289</v>
       </c>
@@ -15068,7 +15080,7 @@
         <v>1291</v>
       </c>
     </row>
-    <row r="419" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="419" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A419" s="2" t="s">
         <v>1292</v>
       </c>
@@ -15091,7 +15103,7 @@
         <v>1294</v>
       </c>
     </row>
-    <row r="420" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="420" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A420" s="2" t="s">
         <v>1295</v>
       </c>
@@ -15114,7 +15126,7 @@
         <v>1297</v>
       </c>
     </row>
-    <row r="421" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="421" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A421" s="2" t="s">
         <v>1298</v>
       </c>
@@ -15137,7 +15149,7 @@
         <v>1300</v>
       </c>
     </row>
-    <row r="422" spans="1:7" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="422" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A422" s="2" t="s">
         <v>1301</v>
       </c>
@@ -15160,7 +15172,7 @@
         <v>1303</v>
       </c>
     </row>
-    <row r="423" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="423" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A423" s="2" t="s">
         <v>1304</v>
       </c>
@@ -15183,7 +15195,7 @@
         <v>1306</v>
       </c>
     </row>
-    <row r="424" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="424" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A424" s="2" t="s">
         <v>1307</v>
       </c>
@@ -15206,7 +15218,7 @@
         <v>1309</v>
       </c>
     </row>
-    <row r="425" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="425" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A425" s="2" t="s">
         <v>1310</v>
       </c>
@@ -15229,7 +15241,7 @@
         <v>1313</v>
       </c>
     </row>
-    <row r="426" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="426" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A426" s="2" t="s">
         <v>1314</v>
       </c>
@@ -15252,7 +15264,7 @@
         <v>1317</v>
       </c>
     </row>
-    <row r="427" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="427" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A427" s="2" t="s">
         <v>1318</v>
       </c>
@@ -15275,7 +15287,7 @@
         <v>1320</v>
       </c>
     </row>
-    <row r="428" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="428" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A428" s="2" t="s">
         <v>1321</v>
       </c>
@@ -15298,7 +15310,7 @@
         <v>1323</v>
       </c>
     </row>
-    <row r="429" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="429" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A429" s="2" t="s">
         <v>1324</v>
       </c>
@@ -15321,7 +15333,7 @@
         <v>1326</v>
       </c>
     </row>
-    <row r="430" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="430" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A430" s="2" t="s">
         <v>1327</v>
       </c>
@@ -15344,7 +15356,7 @@
         <v>1330</v>
       </c>
     </row>
-    <row r="431" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="431" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A431" s="2" t="s">
         <v>1331</v>
       </c>
@@ -15367,7 +15379,7 @@
         <v>1333</v>
       </c>
     </row>
-    <row r="432" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="432" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A432" s="2" t="s">
         <v>1334</v>
       </c>
@@ -15390,7 +15402,7 @@
         <v>1336</v>
       </c>
     </row>
-    <row r="433" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="433" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A433" s="2" t="s">
         <v>1337</v>
       </c>
@@ -15413,7 +15425,7 @@
         <v>1339</v>
       </c>
     </row>
-    <row r="434" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="434" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A434" s="2" t="s">
         <v>1340</v>
       </c>
@@ -15436,7 +15448,7 @@
         <v>1342</v>
       </c>
     </row>
-    <row r="435" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="435" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A435" s="2" t="s">
         <v>1343</v>
       </c>
@@ -15459,7 +15471,7 @@
         <v>1345</v>
       </c>
     </row>
-    <row r="436" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="436" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A436" s="2" t="s">
         <v>1346</v>
       </c>
@@ -15482,7 +15494,7 @@
         <v>1348</v>
       </c>
     </row>
-    <row r="437" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="437" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A437" s="2" t="s">
         <v>1349</v>
       </c>
@@ -15505,7 +15517,7 @@
         <v>1351</v>
       </c>
     </row>
-    <row r="438" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="438" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A438" s="2" t="s">
         <v>1352</v>
       </c>
@@ -15528,7 +15540,7 @@
         <v>1354</v>
       </c>
     </row>
-    <row r="439" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="439" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A439" s="2" t="s">
         <v>1355</v>
       </c>
@@ -15551,7 +15563,7 @@
         <v>1357</v>
       </c>
     </row>
-    <row r="440" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="440" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A440" s="2" t="s">
         <v>1358</v>
       </c>
@@ -15574,7 +15586,7 @@
         <v>1361</v>
       </c>
     </row>
-    <row r="441" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="441" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A441" s="2" t="s">
         <v>1362</v>
       </c>
@@ -15597,7 +15609,7 @@
         <v>1364</v>
       </c>
     </row>
-    <row r="442" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="442" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A442" s="2" t="s">
         <v>1365</v>
       </c>
@@ -15620,7 +15632,7 @@
         <v>1367</v>
       </c>
     </row>
-    <row r="443" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="443" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A443" s="2" t="s">
         <v>1368</v>
       </c>
@@ -15643,7 +15655,7 @@
         <v>1370</v>
       </c>
     </row>
-    <row r="444" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="444" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A444" s="2" t="s">
         <v>1371</v>
       </c>
@@ -15666,7 +15678,7 @@
         <v>1373</v>
       </c>
     </row>
-    <row r="445" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="445" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A445" s="2" t="s">
         <v>1374</v>
       </c>
@@ -15689,7 +15701,7 @@
         <v>1376</v>
       </c>
     </row>
-    <row r="446" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="446" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A446" s="2" t="s">
         <v>1377</v>
       </c>
@@ -15712,7 +15724,7 @@
         <v>1380</v>
       </c>
     </row>
-    <row r="447" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="447" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A447" s="2" t="s">
         <v>1381</v>
       </c>
@@ -15735,7 +15747,7 @@
         <v>1383</v>
       </c>
     </row>
-    <row r="448" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="448" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A448" s="2" t="s">
         <v>1384</v>
       </c>
@@ -15758,7 +15770,7 @@
         <v>1385</v>
       </c>
     </row>
-    <row r="449" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="449" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A449" s="2" t="s">
         <v>1386</v>
       </c>
@@ -15781,7 +15793,7 @@
         <v>1388</v>
       </c>
     </row>
-    <row r="450" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="450" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A450" s="2" t="s">
         <v>1389</v>
       </c>
@@ -15804,7 +15816,7 @@
         <v>1391</v>
       </c>
     </row>
-    <row r="451" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="451" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A451" s="2" t="s">
         <v>1392</v>
       </c>
@@ -15827,7 +15839,7 @@
         <v>1394</v>
       </c>
     </row>
-    <row r="452" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="452" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A452" s="2" t="s">
         <v>1395</v>
       </c>
@@ -15850,7 +15862,7 @@
         <v>1398</v>
       </c>
     </row>
-    <row r="453" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="453" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A453" s="2" t="s">
         <v>1399</v>
       </c>
@@ -15873,7 +15885,7 @@
         <v>1401</v>
       </c>
     </row>
-    <row r="454" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="454" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A454" s="2" t="s">
         <v>1402</v>
       </c>
@@ -15896,7 +15908,7 @@
         <v>1405</v>
       </c>
     </row>
-    <row r="455" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="455" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A455" s="2" t="s">
         <v>1406</v>
       </c>
@@ -15919,7 +15931,7 @@
         <v>1408</v>
       </c>
     </row>
-    <row r="456" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="456" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A456" s="2" t="s">
         <v>1409</v>
       </c>
@@ -15942,7 +15954,7 @@
         <v>1411</v>
       </c>
     </row>
-    <row r="457" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="457" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A457" s="2" t="s">
         <v>1412</v>
       </c>
@@ -15965,7 +15977,7 @@
         <v>1414</v>
       </c>
     </row>
-    <row r="458" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="458" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A458" s="2" t="s">
         <v>1415</v>
       </c>
@@ -15988,7 +16000,7 @@
         <v>1417</v>
       </c>
     </row>
-    <row r="459" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="459" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A459" s="2" t="s">
         <v>1418</v>
       </c>
@@ -16011,7 +16023,7 @@
         <v>1420</v>
       </c>
     </row>
-    <row r="460" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="460" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A460" s="2" t="s">
         <v>1421</v>
       </c>
@@ -16034,7 +16046,7 @@
         <v>1423</v>
       </c>
     </row>
-    <row r="461" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="461" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A461" s="2" t="s">
         <v>1424</v>
       </c>
@@ -16057,7 +16069,7 @@
         <v>1426</v>
       </c>
     </row>
-    <row r="462" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="462" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A462" s="2" t="s">
         <v>1427</v>
       </c>
@@ -16080,7 +16092,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="463" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="463" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A463" s="2" t="s">
         <v>1430</v>
       </c>
@@ -16103,7 +16115,7 @@
         <v>1432</v>
       </c>
     </row>
-    <row r="464" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="464" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A464" s="2" t="s">
         <v>1433</v>
       </c>
@@ -16126,7 +16138,7 @@
         <v>1435</v>
       </c>
     </row>
-    <row r="465" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="465" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A465" s="2" t="s">
         <v>1436</v>
       </c>
@@ -16149,7 +16161,7 @@
         <v>1439</v>
       </c>
     </row>
-    <row r="466" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="466" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A466" s="2" t="s">
         <v>1440</v>
       </c>
@@ -16172,7 +16184,7 @@
         <v>1442</v>
       </c>
     </row>
-    <row r="467" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="467" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A467" s="2" t="s">
         <v>1443</v>
       </c>
@@ -16195,7 +16207,7 @@
         <v>1445</v>
       </c>
     </row>
-    <row r="468" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="468" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A468" s="2" t="s">
         <v>1446</v>
       </c>
@@ -16218,7 +16230,7 @@
         <v>1448</v>
       </c>
     </row>
-    <row r="469" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="469" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A469" s="2" t="s">
         <v>1449</v>
       </c>
@@ -16241,7 +16253,7 @@
         <v>1451</v>
       </c>
     </row>
-    <row r="470" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="470" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A470" s="2" t="s">
         <v>1452</v>
       </c>
@@ -16264,7 +16276,7 @@
         <v>1454</v>
       </c>
     </row>
-    <row r="471" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="471" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A471" s="2" t="s">
         <v>1455</v>
       </c>
@@ -16287,7 +16299,7 @@
         <v>1458</v>
       </c>
     </row>
-    <row r="472" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="472" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A472" s="2" t="s">
         <v>1459</v>
       </c>
@@ -16310,7 +16322,7 @@
         <v>1461</v>
       </c>
     </row>
-    <row r="473" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="473" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A473" s="2" t="s">
         <v>1462</v>
       </c>
@@ -16333,7 +16345,7 @@
         <v>1464</v>
       </c>
     </row>
-    <row r="474" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="474" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A474" s="2" t="s">
         <v>1465</v>
       </c>
@@ -16356,7 +16368,7 @@
         <v>1468</v>
       </c>
     </row>
-    <row r="475" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="475" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A475" s="2" t="s">
         <v>1469</v>
       </c>
@@ -16379,7 +16391,7 @@
         <v>1471</v>
       </c>
     </row>
-    <row r="476" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="476" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A476" s="2" t="s">
         <v>1472</v>
       </c>
@@ -16402,7 +16414,7 @@
         <v>1474</v>
       </c>
     </row>
-    <row r="477" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="477" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A477" s="2" t="s">
         <v>1475</v>
       </c>
@@ -16425,7 +16437,7 @@
         <v>1477</v>
       </c>
     </row>
-    <row r="478" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="478" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A478" s="2" t="s">
         <v>1478</v>
       </c>
@@ -16448,7 +16460,7 @@
         <v>1480</v>
       </c>
     </row>
-    <row r="479" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="479" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A479" s="2" t="s">
         <v>1481</v>
       </c>
@@ -16471,7 +16483,7 @@
         <v>1483</v>
       </c>
     </row>
-    <row r="480" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="480" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A480" s="2" t="s">
         <v>1484</v>
       </c>
@@ -16494,7 +16506,7 @@
         <v>1486</v>
       </c>
     </row>
-    <row r="481" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="481" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A481" s="2" t="s">
         <v>1487</v>
       </c>
@@ -16517,7 +16529,7 @@
         <v>1489</v>
       </c>
     </row>
-    <row r="482" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="482" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A482" s="2" t="s">
         <v>1490</v>
       </c>
@@ -16540,7 +16552,7 @@
         <v>1492</v>
       </c>
     </row>
-    <row r="483" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="483" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A483" s="2" t="s">
         <v>1493</v>
       </c>
@@ -16563,7 +16575,7 @@
         <v>1495</v>
       </c>
     </row>
-    <row r="484" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="484" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A484" s="2" t="s">
         <v>1496</v>
       </c>
@@ -16586,7 +16598,7 @@
         <v>1498</v>
       </c>
     </row>
-    <row r="485" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="485" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A485" s="2" t="s">
         <v>1499</v>
       </c>
@@ -16609,7 +16621,7 @@
         <v>1501</v>
       </c>
     </row>
-    <row r="486" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="486" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A486" s="2" t="s">
         <v>1502</v>
       </c>
@@ -16632,7 +16644,7 @@
         <v>1505</v>
       </c>
     </row>
-    <row r="487" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="487" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A487" s="2" t="s">
         <v>1506</v>
       </c>
@@ -16655,7 +16667,7 @@
         <v>1508</v>
       </c>
     </row>
-    <row r="488" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="488" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A488" s="2" t="s">
         <v>1509</v>
       </c>
@@ -16678,7 +16690,7 @@
         <v>1511</v>
       </c>
     </row>
-    <row r="489" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="489" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A489" s="2" t="s">
         <v>1512</v>
       </c>
@@ -16701,7 +16713,7 @@
         <v>1514</v>
       </c>
     </row>
-    <row r="490" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="490" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A490" s="2" t="s">
         <v>1515</v>
       </c>
@@ -16724,7 +16736,7 @@
         <v>1517</v>
       </c>
     </row>
-    <row r="491" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="491" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A491" s="2" t="s">
         <v>1518</v>
       </c>
@@ -16747,7 +16759,7 @@
         <v>1521</v>
       </c>
     </row>
-    <row r="492" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="492" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A492" s="2" t="s">
         <v>1522</v>
       </c>
@@ -16770,7 +16782,7 @@
         <v>1524</v>
       </c>
     </row>
-    <row r="493" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="493" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A493" s="2" t="s">
         <v>1525</v>
       </c>
@@ -16793,7 +16805,7 @@
         <v>1528</v>
       </c>
     </row>
-    <row r="494" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="494" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A494" s="2" t="s">
         <v>1529</v>
       </c>
@@ -16816,7 +16828,7 @@
         <v>1530</v>
       </c>
     </row>
-    <row r="495" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="495" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A495" s="2" t="s">
         <v>1531</v>
       </c>
@@ -16839,7 +16851,7 @@
         <v>1534</v>
       </c>
     </row>
-    <row r="496" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="496" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A496" s="2" t="s">
         <v>1535</v>
       </c>
@@ -16862,7 +16874,7 @@
         <v>1538</v>
       </c>
     </row>
-    <row r="497" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="497" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A497" s="2" t="s">
         <v>1539</v>
       </c>
@@ -16885,7 +16897,7 @@
         <v>1541</v>
       </c>
     </row>
-    <row r="498" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="498" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A498" s="2" t="s">
         <v>1542</v>
       </c>
@@ -16908,7 +16920,7 @@
         <v>1544</v>
       </c>
     </row>
-    <row r="499" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="499" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A499" s="2" t="s">
         <v>1545</v>
       </c>
@@ -16931,7 +16943,7 @@
         <v>1548</v>
       </c>
     </row>
-    <row r="500" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="500" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A500" s="2" t="s">
         <v>1549</v>
       </c>
@@ -16954,7 +16966,7 @@
         <v>1552</v>
       </c>
     </row>
-    <row r="501" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="501" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A501" s="2" t="s">
         <v>1553</v>
       </c>
@@ -16977,7 +16989,7 @@
         <v>1555</v>
       </c>
     </row>
-    <row r="502" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="502" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A502" s="2" t="s">
         <v>1556</v>
       </c>
@@ -17000,7 +17012,7 @@
         <v>1558</v>
       </c>
     </row>
-    <row r="503" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="503" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A503" s="2" t="s">
         <v>1559</v>
       </c>
@@ -17023,7 +17035,7 @@
         <v>1561</v>
       </c>
     </row>
-    <row r="504" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="504" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A504" s="2" t="s">
         <v>1562</v>
       </c>
@@ -17046,7 +17058,7 @@
         <v>1564</v>
       </c>
     </row>
-    <row r="505" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="505" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A505" s="2" t="s">
         <v>1565</v>
       </c>
@@ -17069,7 +17081,7 @@
         <v>1567</v>
       </c>
     </row>
-    <row r="506" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="506" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A506" s="2" t="s">
         <v>1568</v>
       </c>
@@ -17092,7 +17104,7 @@
         <v>1569</v>
       </c>
     </row>
-    <row r="507" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="507" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A507" s="2" t="s">
         <v>1570</v>
       </c>
@@ -17115,7 +17127,7 @@
         <v>1572</v>
       </c>
     </row>
-    <row r="508" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="508" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A508" s="2" t="s">
         <v>1573</v>
       </c>
@@ -17138,7 +17150,7 @@
         <v>1575</v>
       </c>
     </row>
-    <row r="509" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="509" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A509" s="2" t="s">
         <v>1576</v>
       </c>
@@ -17161,7 +17173,7 @@
         <v>1578</v>
       </c>
     </row>
-    <row r="510" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="510" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A510" s="2" t="s">
         <v>1579</v>
       </c>
@@ -17184,7 +17196,7 @@
         <v>1581</v>
       </c>
     </row>
-    <row r="511" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="511" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A511" s="2" t="s">
         <v>1582</v>
       </c>
@@ -17207,7 +17219,7 @@
         <v>1584</v>
       </c>
     </row>
-    <row r="512" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="512" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A512" s="2" t="s">
         <v>1585</v>
       </c>
@@ -17230,7 +17242,7 @@
         <v>1587</v>
       </c>
     </row>
-    <row r="513" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="513" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A513" s="2" t="s">
         <v>1588</v>
       </c>
@@ -17253,7 +17265,7 @@
         <v>1590</v>
       </c>
     </row>
-    <row r="514" spans="1:7" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="514" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A514" s="2" t="s">
         <v>1591</v>
       </c>
@@ -17276,7 +17288,7 @@
         <v>1593</v>
       </c>
     </row>
-    <row r="515" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="515" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A515" s="2" t="s">
         <v>1594</v>
       </c>
@@ -17299,7 +17311,7 @@
         <v>1596</v>
       </c>
     </row>
-    <row r="516" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="516" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A516" s="2" t="s">
         <v>1597</v>
       </c>
@@ -17322,7 +17334,7 @@
         <v>1599</v>
       </c>
     </row>
-    <row r="517" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="517" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A517" s="2" t="s">
         <v>1600</v>
       </c>
@@ -17345,7 +17357,7 @@
         <v>1602</v>
       </c>
     </row>
-    <row r="518" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="518" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A518" s="2" t="s">
         <v>1603</v>
       </c>
@@ -17368,7 +17380,7 @@
         <v>1605</v>
       </c>
     </row>
-    <row r="519" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="519" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A519" s="2" t="s">
         <v>1606</v>
       </c>
@@ -17391,7 +17403,7 @@
         <v>1608</v>
       </c>
     </row>
-    <row r="520" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="520" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A520" s="2" t="s">
         <v>1609</v>
       </c>
@@ -17414,7 +17426,7 @@
         <v>1612</v>
       </c>
     </row>
-    <row r="521" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="521" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A521" s="2" t="s">
         <v>1613</v>
       </c>
@@ -17437,7 +17449,7 @@
         <v>1615</v>
       </c>
     </row>
-    <row r="522" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="522" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A522" s="2" t="s">
         <v>1616</v>
       </c>
@@ -17460,7 +17472,7 @@
         <v>1618</v>
       </c>
     </row>
-    <row r="523" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="523" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A523" s="2" t="s">
         <v>1619</v>
       </c>
@@ -17483,7 +17495,7 @@
         <v>1621</v>
       </c>
     </row>
-    <row r="524" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="524" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A524" s="2" t="s">
         <v>1622</v>
       </c>
@@ -17506,7 +17518,7 @@
         <v>1624</v>
       </c>
     </row>
-    <row r="525" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="525" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A525" s="2" t="s">
         <v>1625</v>
       </c>
@@ -17529,7 +17541,7 @@
         <v>1627</v>
       </c>
     </row>
-    <row r="526" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="526" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A526" s="2" t="s">
         <v>1628</v>
       </c>
@@ -17552,7 +17564,7 @@
         <v>1630</v>
       </c>
     </row>
-    <row r="527" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="527" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A527" s="2" t="s">
         <v>1631</v>
       </c>
@@ -17575,7 +17587,7 @@
         <v>1633</v>
       </c>
     </row>
-    <row r="528" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="528" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A528" s="2" t="s">
         <v>1634</v>
       </c>
@@ -17598,7 +17610,7 @@
         <v>1636</v>
       </c>
     </row>
-    <row r="529" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="529" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A529" s="2" t="s">
         <v>1637</v>
       </c>
@@ -17621,7 +17633,7 @@
         <v>1639</v>
       </c>
     </row>
-    <row r="530" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="530" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A530" s="2" t="s">
         <v>1640</v>
       </c>
@@ -17644,7 +17656,7 @@
         <v>1642</v>
       </c>
     </row>
-    <row r="531" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="531" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A531" s="2" t="s">
         <v>1643</v>
       </c>
@@ -17667,7 +17679,7 @@
         <v>1645</v>
       </c>
     </row>
-    <row r="532" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="532" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A532" s="2" t="s">
         <v>1646</v>
       </c>
@@ -17690,7 +17702,7 @@
         <v>1648</v>
       </c>
     </row>
-    <row r="533" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="533" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A533" s="2" t="s">
         <v>1649</v>
       </c>
@@ -17713,7 +17725,7 @@
         <v>1652</v>
       </c>
     </row>
-    <row r="534" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="534" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A534" s="2" t="s">
         <v>1653</v>
       </c>
@@ -17736,7 +17748,7 @@
         <v>1656</v>
       </c>
     </row>
-    <row r="535" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="535" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A535" s="2" t="s">
         <v>1657</v>
       </c>
@@ -17759,7 +17771,7 @@
         <v>1660</v>
       </c>
     </row>
-    <row r="536" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="536" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A536" s="2" t="s">
         <v>1661</v>
       </c>
@@ -17782,7 +17794,7 @@
         <v>1663</v>
       </c>
     </row>
-    <row r="537" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="537" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A537" s="2" t="s">
         <v>1664</v>
       </c>
@@ -17805,7 +17817,7 @@
         <v>1666</v>
       </c>
     </row>
-    <row r="538" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="538" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A538" s="2" t="s">
         <v>1667</v>
       </c>
@@ -17828,7 +17840,7 @@
         <v>1669</v>
       </c>
     </row>
-    <row r="539" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="539" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A539" s="2" t="s">
         <v>1670</v>
       </c>
@@ -17851,7 +17863,7 @@
         <v>1672</v>
       </c>
     </row>
-    <row r="540" spans="1:7" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="540" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A540" s="2" t="s">
         <v>1673</v>
       </c>
@@ -17874,7 +17886,7 @@
         <v>1675</v>
       </c>
     </row>
-    <row r="541" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="541" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A541" s="2" t="s">
         <v>1676</v>
       </c>
@@ -17898,13 +17910,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:G541" xr:uid="{00000000-0009-0000-0000-000000000000}">
-    <filterColumn colId="4">
-      <filters>
-        <filter val="AVDA EL CANAL 19591, KM. 12,5 ruta 68"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:G541" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>